<commit_message>
formatting the spread sheet to even out rows and columns
</commit_message>
<xml_diff>
--- a/Assignments/Assignment_14/User Story Specs.xlsx
+++ b/Assignments/Assignment_14/User Story Specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/this-sam-pugh/Desktop/Git_Repos/CS3398-Kree-F2019/Assignments/Assignment_14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C022B086-94CE-7A40-9DA5-98939C18C16B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6DC27D0-8FF3-D140-9F97-D8C296A69505}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17880" yWindow="460" windowWidth="23040" windowHeight="14600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -245,7 +245,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -385,11 +385,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -442,6 +455,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -828,7 +844,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A5"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -917,7 +933,7 @@
     </row>
     <row r="5" spans="1:10" ht="183" customHeight="1" thickBot="1">
       <c r="A5" s="15"/>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="21" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="12"/>
@@ -927,7 +943,7 @@
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
     </row>
-    <row r="6" spans="1:10" ht="17" thickBot="1">
+    <row r="6" spans="1:10" ht="200" customHeight="1" thickBot="1">
       <c r="A6" s="15"/>
       <c r="B6" s="10" t="s">
         <v>12</v>
@@ -941,7 +957,7 @@
     </row>
     <row r="7" spans="1:10" ht="181" customHeight="1" thickBot="1">
       <c r="A7" s="15"/>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="21" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="12"/>
@@ -965,7 +981,7 @@
     </row>
     <row r="9" spans="1:10" ht="200" customHeight="1">
       <c r="A9" s="15"/>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="21" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="12"/>
@@ -989,7 +1005,7 @@
     </row>
     <row r="11" spans="1:10" ht="200" customHeight="1">
       <c r="A11" s="15"/>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="21" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="12"/>
@@ -1013,7 +1029,7 @@
     </row>
     <row r="13" spans="1:10" ht="223.75" customHeight="1">
       <c r="A13" s="15"/>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="12"/>

</xml_diff>

<commit_message>
adding Sam User Stories to speadsheet for assingment 14
</commit_message>
<xml_diff>
--- a/Assignments/Assignment_14/User Story Specs.xlsx
+++ b/Assignments/Assignment_14/User Story Specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/this-sam-pugh/Desktop/Git_Repos/CS3398-Kree-F2019/Assignments/Assignment_14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6DC27D0-8FF3-D140-9F97-D8C296A69505}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50CBA36E-679A-4743-8AEA-2451C7A6A117}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17880" yWindow="460" windowWidth="23040" windowHeight="14600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>Project User Stories and Functional Requirements</t>
   </si>
@@ -119,6 +119,34 @@
   </si>
   <si>
     <t>List Team Members Here: Shelby Jordan, David Kim, Sam Pugh, Ben Kowacki, Jesse Munoz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. I, As a User of this application, Would like to have compelling and easy to navigate drop down menu's which are styled and colored in a mannor that makes them easy to discern and understand. 
+2. I, As a User, I would like the parking information to be displayed in a mannor that is easy for me to understand and interpret. EG, When a button is clicked, the information displayed in a clear and concise mannor. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. A Tabular display format that makes manipulation of the data columns easy for the programmer and attractive to the consumer. 
+2. Propper Headings to go with each of the various fields within the table. </t>
+  </si>
+  <si>
+    <t>1. An Easy to understand color scheme relevant to the map we have built.
+2. Well Built and placed within the page to allow space for the rather large Drop Down Columns.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Color Coded according to permit type or availablity.
+2. ability to display all the information that we have stored in the database to the user. </t>
+  </si>
+  <si>
+    <t>1. A Well Styled Drop down to distinguish it from the other buttonts/elements on the page. 
+2. Ability for user to reset Options Clicked by either re clicking the option or clicking a reset button for the entire page.</t>
+  </si>
+  <si>
+    <t>1. Optional Buttons Such as Go Back to remove last clicked elements without effecting the rest of the data.
+2. JavaScript Error handling and logging for errors and bugs that occiur between the fron end buttons and back end controller.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Additional Links within the displayed data to refer them to another page of the txstate website with more up to date information. 
+2. Backend Controls to verify information has enough space in filed and it will not cause veiwing issues on the page. </t>
   </si>
 </sst>
 </file>
@@ -245,7 +273,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -380,19 +408,6 @@
         <color auto="1"/>
       </right>
       <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -402,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -429,9 +444,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -456,7 +468,13 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -843,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -861,42 +879,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="4" customFormat="1" ht="40">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
       <c r="I1" s="2"/>
       <c r="J1" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="5" customFormat="1" ht="22" customHeight="1">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="20" t="s">
+      <c r="D2" s="18"/>
+      <c r="E2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
     </row>
     <row r="3" spans="1:10" s="5" customFormat="1" ht="16" customHeight="1">
-      <c r="A3" s="17"/>
-      <c r="B3" s="18"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="17"/>
       <c r="C3" s="6" t="s">
         <v>4</v>
       </c>
@@ -919,125 +937,139 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="103" customHeight="1">
-      <c r="A4" s="15"/>
+    <row r="4" spans="1:10" ht="200" customHeight="1">
+      <c r="A4" s="14"/>
       <c r="B4" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
     </row>
     <row r="5" spans="1:10" ht="183" customHeight="1" thickBot="1">
-      <c r="A5" s="15"/>
-      <c r="B5" s="21" t="s">
+      <c r="A5" s="14"/>
+      <c r="B5" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="200" customHeight="1" thickBot="1">
-      <c r="A6" s="15"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:10" ht="181" customHeight="1" thickBot="1">
-      <c r="A7" s="15"/>
-      <c r="B7" s="21" t="s">
+      <c r="A7" s="14"/>
+      <c r="B7" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-    </row>
-    <row r="8" spans="1:10" ht="189" customHeight="1" thickBot="1">
-      <c r="A8" s="15"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+    </row>
+    <row r="8" spans="1:10" ht="250" customHeight="1" thickBot="1">
+      <c r="A8" s="14" t="s">
+        <v>18</v>
+      </c>
       <c r="B8" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-    </row>
-    <row r="9" spans="1:10" ht="200" customHeight="1">
-      <c r="A9" s="15"/>
-      <c r="B9" s="21" t="s">
+      <c r="E8" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="13"/>
+    </row>
+    <row r="9" spans="1:10" ht="250" customHeight="1">
+      <c r="A9" s="14"/>
+      <c r="B9" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:10" ht="200" customHeight="1">
-      <c r="A10" s="15"/>
+      <c r="A10" s="14"/>
       <c r="B10" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:10" ht="200" customHeight="1">
-      <c r="A11" s="15"/>
-      <c r="B11" s="21" t="s">
+      <c r="A11" s="14"/>
+      <c r="B11" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
     </row>
     <row r="12" spans="1:10" ht="181.25" customHeight="1">
-      <c r="A12" s="15"/>
+      <c r="A12" s="14"/>
       <c r="B12" s="10" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:10" ht="223.75" customHeight="1">
-      <c r="A13" s="15"/>
-      <c r="B13" s="21" t="s">
+      <c r="A13" s="14"/>
+      <c r="B13" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>

<commit_message>
adding shelby's updates to spreadsheet in repo
</commit_message>
<xml_diff>
--- a/Assignments/Assignment_14/User Story Specs.xlsx
+++ b/Assignments/Assignment_14/User Story Specs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BenVR\Documents\GitHub\CS3398-Kree-F2019\Assignments\Assignment_14\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/this-sam-pugh/Desktop/Git_Repos/CS3398-Kree-F2019/Assignments/Assignment_14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54AC2BC4-12B3-44A6-86B0-8C24ACC722A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4780C5-7C64-BA4E-8893-F8D201C8604F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="15796" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8720" yWindow="6020" windowWidth="16880" windowHeight="9040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
   <si>
     <t>Project User Stories and Functional Requirements</t>
   </si>
@@ -242,12 +242,38 @@
   <si>
     <t>2. As a student, I would like to be able to put in my schedule and have the website tell me what time to arrive for the best chance to get a parking spot.</t>
   </si>
+  <si>
+    <t>As a user, i would like the ability to discern which parking lots have more parking spaces than others depending on my anticipated arrival time.</t>
+  </si>
+  <si>
+    <t>1. An option for the user to select their expected arrival time.
+2. A legend so that the user can distinguish lot availability.</t>
+  </si>
+  <si>
+    <t>1. A clearly identifiable area to input the expected time of arrival.
+2. A hover over lot window that displays the lot information at that time.</t>
+  </si>
+  <si>
+    <t>1. A backend function that predicts the available lots based on a user input time and only displays those.
+2. A hover over lot window that displays the lot information at that time.</t>
+  </si>
+  <si>
+    <t>As a user, I would like the option to select multiple parking options simultaneously and determine my anticipated desitination so that I can see which lot provides the best walking option to my classes.</t>
+  </si>
+  <si>
+    <t>1. A dropdown selection that is filtered by available lots.
+2.A clear walking path and some way to distinguish between multiple options.</t>
+  </si>
+  <si>
+    <t>1. Color coded paths.
+2.A table or some other form that shows all parking options the user selected.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -291,6 +317,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF262626"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -511,7 +543,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -556,6 +588,12 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -571,8 +609,17 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -958,60 +1005,60 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.765625" defaultRowHeight="14.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="41.3046875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.4609375" customWidth="1"/>
-    <col min="3" max="3" width="16.69140625" customWidth="1"/>
-    <col min="4" max="4" width="13.4609375" customWidth="1"/>
-    <col min="5" max="5" width="15.4609375" customWidth="1"/>
+    <col min="1" max="1" width="41.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="16.765625" customWidth="1"/>
-    <col min="10" max="10" width="49.3046875" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" customWidth="1"/>
+    <col min="10" max="10" width="49.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" ht="55.3">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:10" s="4" customFormat="1" ht="40">
+      <c r="A1" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
       <c r="I1" s="2"/>
       <c r="J1" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="5" customFormat="1" ht="22.1" customHeight="1">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:10" s="5" customFormat="1" ht="22" customHeight="1">
+      <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="22" t="s">
+      <c r="D2" s="23"/>
+      <c r="E2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
     </row>
-    <row r="3" spans="1:10" s="5" customFormat="1" ht="16.100000000000001" customHeight="1">
-      <c r="A3" s="19"/>
-      <c r="B3" s="20"/>
+    <row r="3" spans="1:10" s="5" customFormat="1" ht="16" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A3" s="21"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="6" t="s">
         <v>4</v>
       </c>
@@ -1034,32 +1081,46 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="199.95" customHeight="1">
-      <c r="A4" s="23"/>
-      <c r="B4" s="10" t="s">
+    <row r="4" spans="1:10" ht="200" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A4" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="25" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
+      <c r="E4" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="H4" s="13"/>
     </row>
     <row r="5" spans="1:10" ht="183" customHeight="1" thickBot="1">
-      <c r="A5" s="23"/>
-      <c r="B5" s="14" t="s">
+      <c r="A5" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="27" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
+      <c r="E5" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="28"/>
       <c r="H5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="199.95" customHeight="1" thickBot="1">
-      <c r="A6" s="23" t="s">
+    <row r="6" spans="1:10" ht="200" customHeight="1" thickBot="1">
+      <c r="A6" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -1078,8 +1139,8 @@
       </c>
       <c r="H6" s="13"/>
     </row>
-    <row r="7" spans="1:10" ht="181.1" customHeight="1" thickBot="1">
-      <c r="A7" s="23"/>
+    <row r="7" spans="1:10" ht="181" customHeight="1" thickBot="1">
+      <c r="A7" s="19"/>
       <c r="B7" s="16" t="s">
         <v>12</v>
       </c>
@@ -1096,8 +1157,8 @@
       </c>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:10" ht="250.1" customHeight="1" thickBot="1">
-      <c r="A8" s="23" t="s">
+    <row r="8" spans="1:10" ht="250" customHeight="1" thickBot="1">
+      <c r="A8" s="19" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -1116,8 +1177,8 @@
       </c>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:10" ht="250.1" customHeight="1" thickBot="1">
-      <c r="A9" s="23"/>
+    <row r="9" spans="1:10" ht="250" customHeight="1" thickBot="1">
+      <c r="A9" s="19"/>
       <c r="B9" s="14" t="s">
         <v>13</v>
       </c>
@@ -1134,7 +1195,7 @@
       </c>
       <c r="H9" s="12"/>
     </row>
-    <row r="10" spans="1:10" ht="199.95" customHeight="1" thickBot="1">
+    <row r="10" spans="1:10" ht="200" customHeight="1" thickBot="1">
       <c r="A10" s="17" t="s">
         <v>49</v>
       </c>
@@ -1156,7 +1217,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="199.95" customHeight="1" thickBot="1">
+    <row r="11" spans="1:10" ht="200" customHeight="1" thickBot="1">
       <c r="A11" s="17" t="s">
         <v>50</v>
       </c>
@@ -1178,8 +1239,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="181.2" customHeight="1" thickBot="1">
-      <c r="A12" s="23" t="s">
+    <row r="12" spans="1:10" ht="181.25" customHeight="1" thickBot="1">
+      <c r="A12" s="19" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -1200,8 +1261,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="223.85" customHeight="1">
-      <c r="A13" s="23"/>
+    <row r="13" spans="1:10" ht="223.75" customHeight="1">
+      <c r="A13" s="19"/>
       <c r="B13" s="14" t="s">
         <v>15</v>
       </c>
@@ -1221,8 +1282,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A4:A5"/>
+  <mergeCells count="8">
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A12:A13"/>

</xml_diff>

<commit_message>
adding spreadsheet with planning poker ideas for assignment 14 to repo
</commit_message>
<xml_diff>
--- a/Assignments/Assignment_14/User Story Specs.xlsx
+++ b/Assignments/Assignment_14/User Story Specs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/this-sam-pugh/Desktop/Git_Repos/CS3398-Kree-F2019/Assignments/Assignment_14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4780C5-7C64-BA4E-8893-F8D201C8604F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA57D21-75E4-244D-AA75-E5A33BA4194C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8720" yWindow="6020" windowWidth="16880" windowHeight="9040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12760" windowHeight="16000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -591,6 +591,18 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -608,18 +620,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1005,8 +1005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B5"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1023,42 +1023,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="4" customFormat="1" ht="40">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
       <c r="I1" s="2"/>
       <c r="J1" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="5" customFormat="1" ht="22" customHeight="1">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="24" t="s">
+      <c r="D2" s="27"/>
+      <c r="E2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:10" s="5" customFormat="1" ht="16" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A3" s="21"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="26"/>
       <c r="C3" s="6" t="s">
         <v>4</v>
       </c>
@@ -1085,18 +1085,22 @@
       <c r="A4" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
+      <c r="C4" s="11">
+        <v>21</v>
+      </c>
+      <c r="D4" s="11">
+        <v>21</v>
+      </c>
       <c r="E4" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="20" t="s">
         <v>54</v>
       </c>
       <c r="H4" s="13"/>
@@ -1105,29 +1109,37 @@
       <c r="A5" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="28" t="s">
+      <c r="C5" s="15">
+        <v>34</v>
+      </c>
+      <c r="D5" s="15">
+        <v>34</v>
+      </c>
+      <c r="E5" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="F5" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="G5" s="28"/>
+      <c r="G5" s="22"/>
       <c r="H5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="200" customHeight="1" thickBot="1">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="23" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
+      <c r="C6" s="11">
+        <v>34</v>
+      </c>
+      <c r="D6" s="11">
+        <v>34</v>
+      </c>
       <c r="E6" s="13" t="s">
         <v>28</v>
       </c>
@@ -1140,12 +1152,16 @@
       <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:10" ht="181" customHeight="1" thickBot="1">
-      <c r="A7" s="19"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
+      <c r="C7" s="15">
+        <v>34</v>
+      </c>
+      <c r="D7" s="15">
+        <v>34</v>
+      </c>
       <c r="E7" s="13" t="s">
         <v>29</v>
       </c>
@@ -1158,14 +1174,18 @@
       <c r="H7" s="13"/>
     </row>
     <row r="8" spans="1:10" ht="250" customHeight="1" thickBot="1">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="23" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
+      <c r="C8" s="11">
+        <v>21</v>
+      </c>
+      <c r="D8" s="11">
+        <v>21</v>
+      </c>
       <c r="E8" s="13" t="s">
         <v>20</v>
       </c>
@@ -1178,12 +1198,16 @@
       <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:10" ht="250" customHeight="1" thickBot="1">
-      <c r="A9" s="19"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
+      <c r="C9" s="15">
+        <v>34</v>
+      </c>
+      <c r="D9" s="15">
+        <v>21</v>
+      </c>
       <c r="E9" s="12" t="s">
         <v>19</v>
       </c>
@@ -1202,8 +1226,12 @@
       <c r="B10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
+      <c r="C10" s="11">
+        <v>34</v>
+      </c>
+      <c r="D10" s="11">
+        <v>89</v>
+      </c>
       <c r="E10" s="13" t="s">
         <v>41</v>
       </c>
@@ -1224,8 +1252,12 @@
       <c r="B11" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
+      <c r="C11" s="15">
+        <v>34</v>
+      </c>
+      <c r="D11" s="15">
+        <v>55</v>
+      </c>
       <c r="E11" s="12" t="s">
         <v>45</v>
       </c>
@@ -1240,14 +1272,18 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="181.25" customHeight="1" thickBot="1">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="23" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
+      <c r="C12" s="11">
+        <v>55</v>
+      </c>
+      <c r="D12" s="11">
+        <v>21</v>
+      </c>
       <c r="E12" s="13" t="s">
         <v>33</v>
       </c>
@@ -1262,12 +1298,16 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="223.75" customHeight="1">
-      <c r="A13" s="19"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
+      <c r="C13" s="15">
+        <v>55</v>
+      </c>
+      <c r="D13" s="15">
+        <v>55</v>
+      </c>
       <c r="E13" s="12" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
adding shelby's updates to spreadsheet
</commit_message>
<xml_diff>
--- a/Assignments/Assignment_14/User Story Specs.xlsx
+++ b/Assignments/Assignment_14/User Story Specs.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/this-sam-pugh/Desktop/Git_Repos/CS3398-Kree-F2019/Assignments/Assignment_14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA57D21-75E4-244D-AA75-E5A33BA4194C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484AB970-5F62-3D4A-9421-A5D314DA426A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12760" windowHeight="16000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="12760" windowHeight="14600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="61">
   <si>
     <t>Project User Stories and Functional Requirements</t>
   </si>
@@ -267,6 +267,18 @@
   <si>
     <t>1. Color coded paths.
 2.A table or some other form that shows all parking options the user selected.</t>
+  </si>
+  <si>
+    <t>1. Pop up options.
+2. Voice interaction.</t>
+  </si>
+  <si>
+    <t>1. Additional routes shown that the user didn’t select.
+2.Show impediments on any route.</t>
+  </si>
+  <si>
+    <t>1.A small window.
+2. A free text area to accept user input for this field.</t>
   </si>
 </sst>
 </file>
@@ -588,20 +600,20 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1005,8 +1017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1082,10 +1094,10 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="200" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="18" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="11">
@@ -1097,19 +1109,21 @@
       <c r="E4" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="13"/>
+      <c r="H4" s="19" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="5" spans="1:10" ht="183" customHeight="1" thickBot="1">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="20" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="15">
@@ -1118,14 +1132,18 @@
       <c r="D5" s="15">
         <v>34</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="G5" s="22"/>
-      <c r="H5" s="12"/>
+      <c r="G5" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="200" customHeight="1" thickBot="1">
       <c r="A6" s="23" t="s">

</xml_diff>

<commit_message>
adding should not have field data for assignment 14 spreadsheet
</commit_message>
<xml_diff>
--- a/Assignments/Assignment_14/User Story Specs.xlsx
+++ b/Assignments/Assignment_14/User Story Specs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/this-sam-pugh/Desktop/Git_Repos/CS3398-Kree-F2019/Assignments/Assignment_14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484AB970-5F62-3D4A-9421-A5D314DA426A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CBA1CF-1459-D14C-B6A1-B1E2307A3AA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="12760" windowHeight="14600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30520" windowHeight="17560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
   <si>
     <t>Project User Stories and Functional Requirements</t>
   </si>
@@ -279,6 +279,14 @@
   <si>
     <t>1.A small window.
 2. A free text area to accept user input for this field.</t>
+  </si>
+  <si>
+    <t>1. Broken Links within the drop down that do not cause reaction on the page.
+2. Links that are not relevant to the groups within the drop downs.</t>
+  </si>
+  <si>
+    <t>1. Information other than what is required in the table. Simplify what the user sees.
+2. Differing color scheme to conflict with the rest of the page.</t>
   </si>
 </sst>
 </file>
@@ -1017,8 +1025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1213,7 +1221,9 @@
       <c r="G8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="13"/>
+      <c r="H8" s="13" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="250" customHeight="1" thickBot="1">
       <c r="A9" s="23"/>
@@ -1235,7 +1245,9 @@
       <c r="G9" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="12"/>
+      <c r="H9" s="12" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="200" customHeight="1" thickBot="1">
       <c r="A10" s="17" t="s">

</xml_diff>